<commit_message>
starting tone generation work
</commit_message>
<xml_diff>
--- a/Calculation Stuff/current consumption.xlsx
+++ b/Calculation Stuff/current consumption.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24301"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\GitHub\FlipClock\Calculation Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9977a44478b21da/Documents/GitHub/FlipClock/Calculation Stuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CD4308-5D47-4771-8BE4-4A2754D9D0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{26FF4A7F-A7DD-4012-8AE6-730F92B80BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8DA1653-FDA3-4E2D-969A-D6106499F343}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-6285" windowWidth="29040" windowHeight="15990" xr2:uid="{F2A7BAD6-DD20-41CC-8C57-8982E7BCC7D6}"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="28800" windowHeight="15555" xr2:uid="{F2A7BAD6-DD20-41CC-8C57-8982E7BCC7D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Number</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>ampm</t>
-  </si>
-  <si>
-    <t>clock</t>
   </si>
   <si>
     <t>total</t>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>Other Main PCB Stuff</t>
+  </si>
+  <si>
+    <t>alarm</t>
   </si>
 </sst>
 </file>
@@ -8185,10 +8185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9B593B-5E26-46FB-A77D-A311D55ABD4C}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8196,12 +8196,12 @@
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8210,7 +8210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -8229,8 +8229,12 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>14*B4</f>
+        <v>0.72666666666666679</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8241,12 +8245,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -8255,16 +8259,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <f>B12*4</f>
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -8272,7 +8276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -8280,9 +8284,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -8290,7 +8294,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <f>SUM(B13:B16)</f>
@@ -8299,7 +8303,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <f>B17*B4</f>
@@ -8311,7 +8315,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>0.2</v>
@@ -8319,12 +8323,27 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f>B22+B21+B20+B18</f>
+        <v>5.5066666666666677</v>
       </c>
     </row>
   </sheetData>
@@ -8356,22 +8375,22 @@
         <v>15</v>
       </c>
       <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
       <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
         <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
       </c>
       <c r="Q1" t="s">
         <v>1</v>
       </c>
       <c r="R1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -8548,7 +8567,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
         <f>60-B7</f>
@@ -8584,7 +8603,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1">
         <f>60-B7</f>
@@ -8663,7 +8682,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2">
         <f>B3/B5</f>
@@ -8719,7 +8738,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
         <v>15</v>
@@ -8751,7 +8770,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1">
         <v>12</v>
@@ -8760,7 +8779,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K15">
         <v>1.4</v>
@@ -8786,21 +8805,21 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="2">
         <f>_xlfn.XLOOKUP(B15,L2:L73,K2:K73,,1,1)</f>
         <v>2.1</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <f>B16*B26</f>
         <v>14.700000000000001</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N16">
         <v>0.15</v>
@@ -8812,21 +8831,21 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1">
         <f>B16</f>
         <v>2.1</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <f>B17*B26</f>
         <v>14.700000000000001</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K17">
         <v>1.5</v>
@@ -8875,7 +8894,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2">
         <f>_xlfn.XLOOKUP(B9,R2:R73,Q2:Q73,,-1,-1)</f>
@@ -8908,7 +8927,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -8940,7 +8959,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2">
         <f>_xlfn.XLOOKUP(B20,Q2:Q73,R2:R73,,-1,-1)</f>
@@ -9019,7 +9038,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>2.7</v>
@@ -9048,7 +9067,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25">
         <v>0.2</v>
@@ -9077,7 +9096,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <f>CEILING(B14/(B24*(1-B25)),1)</f>
@@ -9130,7 +9149,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -9139,7 +9158,7 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K28">
         <v>2.6</v>
@@ -9165,7 +9184,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29">
         <f>B28/(B14/B12)</f>
@@ -9195,7 +9214,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30">
         <f>B29/B26</f>
@@ -17579,7 +17598,7 @@
         <v>46.3</v>
       </c>
       <c r="R465">
-        <f t="shared" ref="R465:R528" si="21">$B$17*($B$14-$B$15)/Q465</f>
+        <f t="shared" ref="R465:R501" si="21">$B$17*($B$14-$B$15)/Q465</f>
         <v>0.13606911447084236</v>
       </c>
     </row>
@@ -18407,7 +18426,7 @@
         <v>52.700000000000202</v>
       </c>
       <c r="L529">
-        <f t="shared" ref="L529:L592" si="22">$B$14*EXP(-$B$7/($B$12*K529))</f>
+        <f t="shared" ref="L529:L558" si="22">$B$14*EXP(-$B$7/($B$12*K529))</f>
         <v>14.872461801394328</v>
       </c>
     </row>

</xml_diff>